<commit_message>
developed improvements in CompareData workflow
</commit_message>
<xml_diff>
--- a/MockData/Mock Data.xlsx
+++ b/MockData/Mock Data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27311"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E58EB636-8E2E-49B8-8B50-5AA6A81469FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{074A3231-38FF-4521-93A3-47839570C7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerData" sheetId="1" r:id="rId1"/>
-    <sheet name="LandTaxAssessments" sheetId="2" r:id="rId2"/>
+    <sheet name="Assessments" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>ClientID</t>
   </si>
@@ -40,6 +40,12 @@
     <t>ClientName</t>
   </si>
   <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
     <t>Address</t>
   </si>
   <si>
@@ -55,6 +61,12 @@
     <t>Sarah Jones</t>
   </si>
   <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
     <t>4 Hope Street HOPEVILLE NSW 2222</t>
   </si>
   <si>
@@ -64,6 +76,12 @@
     <t>Susan Williams</t>
   </si>
   <si>
+    <t>Susan</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
     <t>123 Fake St SYDNEY NSW 2000</t>
   </si>
   <si>
@@ -73,13 +91,34 @@
     <t>Jane Smith</t>
   </si>
   <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
     <t>123 Teal St EASTWOOD NSW 2122</t>
   </si>
   <si>
     <t>janesmith123@gmail.com</t>
   </si>
   <si>
-    <t>CorrespondenceID</t>
+    <t>John Citizen</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Citizen</t>
+  </si>
+  <si>
+    <t>CENTENNIAL PLAZA 260 ELIZABETH ST SURRY HILLS 2010 NSW</t>
+  </si>
+  <si>
+    <t>johncitizen123@gmail.com</t>
+  </si>
+  <si>
+    <t>CorrespondenceID (AssessmentID from CM)</t>
   </si>
   <si>
     <t>AssessmentType</t>
@@ -116,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +173,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -158,13 +204,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,21 +526,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -512,65 +562,115 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>52454</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1">
         <v>61987654320</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2">
         <v>29561</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>52455</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1">
         <v>61987654321</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2">
         <v>36853</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>52456</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1">
         <v>61987654322</v>
       </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="4">
         <v>35188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>52457</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1">
+        <v>619876543223</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="4">
+        <v>27450</v>
       </c>
     </row>
   </sheetData>
@@ -583,7 +683,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -601,26 +701,26 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>15</v>
+      <c r="B1" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -631,7 +731,7 @@
         <v>1234</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2">
         <v>45566</v>
@@ -655,22 +755,22 @@
         <v>1235</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E3" s="5">
         <v>6973.3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -681,22 +781,22 @@
         <v>1235</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E4" s="5">
         <v>6973.3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>